<commit_message>
D8MT-386. Adapted the template.
</commit_message>
<xml_diff>
--- a/templates/content_type_mapping_template.xlsx
+++ b/templates/content_type_mapping_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="D7 Inventory" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
     <sheet name="MAPPING - ... to Publication (oe_publication)" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="tbl_dest" vbProcedure="false">'MAPPING - ... to Landing page (landing_page)'!$C$2:$I$101</definedName>
+    <definedName function="false" hidden="false" name="tbl_dest" vbProcedure="false">'MAPPING - ... to Landing page (landing_page)'!$C$2:$I$96</definedName>
     <definedName function="false" hidden="false" name="tbl_src" vbProcedure="false">#REF!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="80">
   <si>
     <t xml:space="preserve">COMM - Learning Corner</t>
   </si>
@@ -82,10 +82,10 @@
     <t xml:space="preserve">Field cardinality</t>
   </si>
   <si>
-    <t xml:space="preserve">uuid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UUID</t>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content type</t>
   </si>
   <si>
     <t xml:space="preserve">varchar_ascii</t>
@@ -94,19 +94,61 @@
     <t xml:space="preserve">FALSE</t>
   </si>
   <si>
-    <t xml:space="preserve">langcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Language</t>
-  </si>
-  <si>
     <t xml:space="preserve">TRUE</t>
   </si>
   <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Content type</t>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Page title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varchar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_content_short_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alternative title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_content_navigation_title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navigation title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_content_content_owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNLIMITED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_content_legacy_link/uri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirect link / uri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_content_legacy_link/title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirect link / title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oe_content_legacy_link/options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirect link / options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">News (oe_news)</t>
   </si>
   <si>
     <t xml:space="preserve">revision_timestamp</t>
@@ -118,72 +160,6 @@
     <t xml:space="preserve">int</t>
   </si>
   <si>
-    <t xml:space="preserve">title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Page title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">varchar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_content_short_title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alternative title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_content_navigation_title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Navigation title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_content_content_owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Content owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNLIMITED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_content_legacy_link/uri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirect link / uri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_content_legacy_link/title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirect link / title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_content_legacy_link/options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirect link / options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blob</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paragraphs/target_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Content items / target_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">paragraphs/target_revision_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Content items / target_revision_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">News (oe_news)</t>
-  </si>
-  <si>
     <t xml:space="preserve">body/value</t>
   </si>
   <si>
@@ -278,12 +254,6 @@
   </si>
   <si>
     <t xml:space="preserve">Timeline / body</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oe_timeline/format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Timeline / format</t>
   </si>
   <si>
     <t xml:space="preserve">Publication (oe_publication)</t>
@@ -584,20 +554,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:15"/>
+  <dimension ref="1:10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="6" width="15.234693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="25.4438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.6020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="6" width="25.5561224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.719387755102"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="18.719387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="18.8367346938776"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="7" width="10.1938775510204"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="7" width="13.5612244897959"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="15.1173469387755"/>
@@ -690,7 +659,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>1</v>
@@ -701,19 +670,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>1</v>
@@ -724,22 +693,22 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I5" s="1" t="n">
         <v>1</v>
@@ -747,22 +716,22 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>20</v>
       </c>
       <c r="H6" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1" t="n">
         <v>1</v>
@@ -776,19 +745,19 @@
         <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -799,10 +768,10 @@
         <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>20</v>
@@ -822,10 +791,10 @@
         <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>20</v>
@@ -845,134 +814,19 @@
         <v>37</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>38</v>
+        <v>1</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -991,20 +845,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:24"/>
+  <dimension ref="1:21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="16.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="16.5612244897959"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="6" width="14.8775510204082"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="6" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="18.719387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="18.8367346938776"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="18.719387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="18.8367346938776"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="7" width="10.1938775510204"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="7" width="13.5612244897959"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="15.1173469387755"/>
@@ -1017,7 +871,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C1" s="0"/>
       <c r="D1" s="8"/>
@@ -1097,7 +951,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
@@ -1108,16 +962,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>20</v>
@@ -1131,19 +985,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
@@ -1154,16 +1008,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>20</v>
@@ -1177,19 +1031,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>0</v>
@@ -1200,39 +1054,39 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>20</v>
@@ -1246,42 +1100,42 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>38</v>
+      <c r="I10" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>0</v>
@@ -1292,39 +1146,39 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>20</v>
@@ -1338,19 +1192,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>52</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>0</v>
@@ -1361,39 +1215,39 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>38</v>
+      <c r="I15" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>20</v>
@@ -1401,22 +1255,22 @@
       <c r="H16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="1" t="n">
-        <v>1</v>
+      <c r="I16" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>20</v>
@@ -1424,68 +1278,68 @@
       <c r="H17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="1" t="n">
-        <v>1</v>
+      <c r="I17" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>20</v>
@@ -1493,99 +1347,30 @@
       <c r="H20" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="1" t="s">
-        <v>38</v>
+      <c r="I20" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G21" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H21" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1" t="n">
+      <c r="I21" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1605,20 +1390,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:21"/>
+  <dimension ref="1:16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.4438775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5612244897959"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9234693877551"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.719387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8367346938776"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.719387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8367346938776"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.1938775510204"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.5612244897959"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.1173469387755"/>
@@ -1630,7 +1415,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C1" s="0"/>
       <c r="D1" s="8"/>
@@ -1710,7 +1495,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
@@ -1721,19 +1506,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
@@ -1744,19 +1529,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
@@ -1767,16 +1552,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>20</v>
@@ -1796,19 +1581,19 @@
         <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,10 +1604,10 @@
         <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>20</v>
@@ -1842,10 +1627,10 @@
         <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>20</v>
@@ -1859,85 +1644,85 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>38</v>
+      <c r="I10" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>20</v>
@@ -1945,22 +1730,22 @@
       <c r="H13" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I13" s="1" t="n">
-        <v>1</v>
+      <c r="I13" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>20</v>
@@ -1968,22 +1753,22 @@
       <c r="H14" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I14" s="1" t="n">
-        <v>1</v>
+      <c r="I14" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>20</v>
@@ -1991,145 +1776,30 @@
       <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>38</v>
+      <c r="I15" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1" t="n">
+      <c r="I16" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2149,20 +1819,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:22"/>
+  <dimension ref="1:17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.4438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3265306122449"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4438775510204"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.5561224489796"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1581632653061"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.719387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8367346938776"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.1938775510204"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.5612244897959"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.1173469387755"/>
@@ -2174,7 +1844,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C1" s="0"/>
       <c r="D1" s="8"/>
@@ -2254,7 +1924,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
@@ -2265,19 +1935,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>0</v>
@@ -2288,19 +1958,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
@@ -2311,16 +1981,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>20</v>
@@ -2340,19 +2010,19 @@
         <v>30</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2363,10 +2033,10 @@
         <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G8" s="11" t="s">
         <v>20</v>
@@ -2386,10 +2056,10 @@
         <v>35</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>20</v>
@@ -2403,85 +2073,85 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>38</v>
+      <c r="I10" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>20</v>
@@ -2495,19 +2165,19 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>0</v>
@@ -2518,62 +2188,62 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>20</v>
@@ -2581,123 +2251,8 @@
       <c r="H17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H21" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>38</v>
+      <c r="I17" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2716,20 +2271,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:20"/>
+  <dimension ref="1:17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.4438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9540816326531"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5612244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.0714285714286"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.5561224489796"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1581632653061"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.719387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8367346938776"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.1938775510204"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.5612244897959"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.1173469387755"/>
@@ -2741,7 +2296,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C1" s="0"/>
       <c r="D1" s="8"/>
@@ -2821,7 +2376,7 @@
         <v>20</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1" t="n">
         <v>0</v>
@@ -2832,16 +2387,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>20</v>
@@ -2855,19 +2410,19 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H5" s="1" t="n">
         <v>0</v>
@@ -2878,16 +2433,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" s="11" t="s">
         <v>20</v>
@@ -2901,19 +2456,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>0</v>
@@ -2924,39 +2479,39 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G9" s="11" t="s">
         <v>20</v>
@@ -2970,88 +2525,88 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>38</v>
+      <c r="I10" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="D12" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>0</v>
@@ -3062,10 +2617,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>19</v>
@@ -3074,53 +2629,53 @@
         <v>20</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>20</v>
       </c>
       <c r="G15" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H16" s="1" t="n">
         <v>0</v>
@@ -3131,93 +2686,24 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G17" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1" t="n">
+      <c r="I17" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
D8MT-386:Added again the Paragraph fields for the content type Landing Page in the CT template.
</commit_message>
<xml_diff>
--- a/templates/content_type_mapping_template.xlsx
+++ b/templates/content_type_mapping_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="995" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="D7 Inventory" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="84">
   <si>
     <t xml:space="preserve">COMM - Learning Corner</t>
   </si>
@@ -148,6 +148,21 @@
     <t xml:space="preserve">blob</t>
   </si>
   <si>
+    <t xml:space="preserve">paragraphs/target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content items / target_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paragraphs/target_revision_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Content items / target_revision_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">News (oe_news)</t>
   </si>
   <si>
@@ -155,9 +170,6 @@
   </si>
   <si>
     <t xml:space="preserve">Revision create time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int</t>
   </si>
   <si>
     <t xml:space="preserve">body/value</t>
@@ -366,7 +378,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -412,6 +424,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -554,19 +578,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:10"/>
+  <dimension ref="1:12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="6" width="15.234693877551"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="6" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.719387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="27.8367346938776"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="18.8367346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="18.9642857142857"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="7" width="10.1938775510204"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="7" width="13.5612244897959"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="15.1173469387755"/>
@@ -827,6 +851,52 @@
       </c>
       <c r="I10" s="1" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C11" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" s="12" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -856,9 +926,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="6" width="16.5612244897959"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="6" width="14.8775510204082"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="6" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="18.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="6" width="18.9642857142857"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="7" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="18.8367346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="18.9642857142857"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="7" width="10.1938775510204"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="7" width="13.5612244897959"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="7" width="15.1173469387755"/>
@@ -871,7 +941,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C1" s="0"/>
       <c r="D1" s="8"/>
@@ -962,13 +1032,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>20</v>
@@ -1123,13 +1193,13 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>21</v>
@@ -1146,10 +1216,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>19</v>
@@ -1169,13 +1239,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>20</v>
@@ -1192,10 +1262,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>19</v>
@@ -1215,10 +1285,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
@@ -1238,10 +1308,10 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
@@ -1261,10 +1331,10 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>24</v>
@@ -1284,10 +1354,10 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C18" s="0" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>38</v>
@@ -1307,10 +1377,10 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C19" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>19</v>
@@ -1330,13 +1400,13 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>21</v>
@@ -1353,13 +1423,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>21</v>
@@ -1401,9 +1471,9 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5612244897959"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9234693877551"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9642857142857"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8367346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.9642857142857"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.1938775510204"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.5612244897959"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.1173469387755"/>
@@ -1415,7 +1485,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C1" s="0"/>
       <c r="D1" s="8"/>
@@ -1644,13 +1714,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>21</v>
@@ -1667,10 +1737,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>19</v>
@@ -1690,10 +1760,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
@@ -1713,10 +1783,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
@@ -1736,10 +1806,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>19</v>
@@ -1759,13 +1829,13 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>21</v>
@@ -1782,13 +1852,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>21</v>
@@ -1827,12 +1897,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4438775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="16.5612244897959"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.5561224489796"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1581632653061"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8367346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.9642857142857"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.1938775510204"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.5612244897959"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.1173469387755"/>
@@ -1844,7 +1913,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C1" s="0"/>
       <c r="D1" s="8"/>
@@ -2073,13 +2142,13 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>21</v>
@@ -2096,10 +2165,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>19</v>
@@ -2119,10 +2188,10 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>19</v>
@@ -2142,13 +2211,13 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>21</v>
@@ -2165,13 +2234,13 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>21</v>
@@ -2188,10 +2257,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>19</v>
@@ -2211,13 +2280,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>21</v>
@@ -2234,13 +2303,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>21</v>
@@ -2273,18 +2342,18 @@
   </sheetPr>
   <dimension ref="1:17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.5612244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.0714285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1989795918367"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.5561224489796"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1581632653061"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.8367346938776"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.9642857142857"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.1938775510204"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.5612244897959"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.1173469387755"/>
@@ -2296,7 +2365,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C1" s="0"/>
       <c r="D1" s="8"/>
@@ -2387,13 +2456,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>20</v>
@@ -2548,10 +2617,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>19</v>
@@ -2571,13 +2640,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>20</v>
@@ -2594,10 +2663,10 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
@@ -2617,10 +2686,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>19</v>
@@ -2640,10 +2709,10 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>19</v>
@@ -2663,13 +2732,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>21</v>
@@ -2686,13 +2755,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C17" s="0" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>21</v>

</xml_diff>